<commit_message>
08 dec changes commit
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BuildPiperTestData.xlsx
+++ b/src/test/resources/testdata/BuildPiperTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2B0D76A1-98C2-451E-ACCE-D469C5F4752E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0BCE96F2-4B05-400F-9C49-3772E0FB6E6D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="4128" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="3456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="RepoIntegrationData" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1:G12"/>
+  <oleSize ref="A1:F5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="242">
   <si>
     <t>username</t>
   </si>
@@ -737,16 +737,22 @@
     <t>web-ui : https://gitlab.com/ot-okts/images/okts-nodejs.git</t>
   </si>
   <si>
-    <t>new-e2e-cluster</t>
-  </si>
-  <si>
-    <t>demo-dev</t>
-  </si>
-  <si>
     <t xml:space="preserve">application </t>
   </si>
   <si>
     <t>RunwithParameterPipeline</t>
+  </si>
+  <si>
+    <t>ManualBuildandDeployHelmService</t>
+  </si>
+  <si>
+    <t>lenskart-poc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://github.com/opstree/OT-Microservices.git</t>
+  </si>
+  <si>
+    <t>community-cluster</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33546052-E966-4F68-882D-901C990EE3E6}">
   <dimension ref="A1:XFD17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18182,6 +18188,71 @@
         <v>32</v>
       </c>
     </row>
+    <row r="7" spans="1:16384" s="25" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG7" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="13" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -18204,9 +18275,10 @@
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{F03D477A-55B9-4E34-B801-A766FBFA0BA9}"/>
     <hyperlink ref="D4" r:id="rId2" display="https://buildpiper-blue.lenskart.com/application/3/environment/135/dashboard" xr:uid="{E07FEE1E-CE62-4AB3-A59D-092D4B899074}"/>
+    <hyperlink ref="G7" r:id="rId3" display="https://github.com/opstree/OT-Microservices.git" xr:uid="{0320C752-8453-4D5C-92C4-FBCEC4364C59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -18214,8 +18286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D07765-B4CA-46F3-9E73-C148767A4C81}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18269,10 +18341,10 @@
         <v>108</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>115</v>
@@ -18633,6 +18705,7 @@
     <row r="18" spans="1:10" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18903,7 +18976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7161A4-3871-41B8-AFD3-D2E01A42417C}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -19699,7 +19772,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>108</v>
@@ -19738,7 +19811,7 @@
         <v>220</v>
       </c>
       <c r="O17" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
12 dec changes Push
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BuildPiperTestData.xlsx
+++ b/src/test/resources/testdata/BuildPiperTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0BCE96F2-4B05-400F-9C49-3772E0FB6E6D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C20F2D9E-EE2B-4A5E-83E2-E37E9E4D8CEC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="3456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="2928" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="RepoIntegrationData" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A1:F5"/>
+  <oleSize ref="A1:G8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="241">
   <si>
     <t>username</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>toEnv</t>
-  </si>
-  <si>
-    <t>Latest</t>
   </si>
   <si>
     <t>ArtifactName</t>
@@ -1227,10 +1224,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1242,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1250,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1259,10 +1256,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1270,19 +1267,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
         <v>95</v>
       </c>
-      <c r="D3" t="s">
-        <v>96</v>
-      </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1290,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1299,10 +1296,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,19 +1307,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
         <v>95</v>
       </c>
-      <c r="D5" t="s">
-        <v>96</v>
-      </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1331,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1361,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33546052-E966-4F68-882D-901C990EE3E6}">
   <dimension ref="A1:XFD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,10 +1397,10 @@
   <sheetData>
     <row r="1" spans="1:16384" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -1487,16 +1484,16 @@
         <v>44</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AE1" s="7" t="s">
         <v>74</v>
       </c>
       <c r="AF1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AG1" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AH1" s="7" t="s">
         <v>31</v>
@@ -1507,22 +1504,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>18</v>
@@ -1543,25 +1540,25 @@
         <v>28</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AH2" s="5" t="s">
         <v>32</v>
@@ -1572,22 +1569,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>18</v>
@@ -1608,25 +1605,25 @@
         <v>28</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>32</v>
@@ -1637,22 +1634,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>223</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>224</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>18</v>
@@ -1673,16 +1670,16 @@
         <v>28</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O4" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P4" s="23" t="s">
         <v>29</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
@@ -1698,13 +1695,13 @@
       <c r="AC4" s="27"/>
       <c r="AD4" s="27"/>
       <c r="AE4" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF4" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG4" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AH4" s="27"/>
       <c r="AI4" s="27"/>
@@ -18063,22 +18060,22 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>110</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>111</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>18</v>
@@ -18099,25 +18096,25 @@
         <v>28</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P5" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE5" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AF5" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG5" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AH5" s="5" t="s">
         <v>32</v>
@@ -18128,22 +18125,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>18</v>
@@ -18164,25 +18161,25 @@
         <v>28</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P6" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE6" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AF6" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG6" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AH6" s="5" t="s">
         <v>32</v>
@@ -18193,22 +18190,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="G7" s="28" t="s">
         <v>239</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>240</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>18</v>
@@ -18229,25 +18226,25 @@
         <v>28</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P7" s="28" t="s">
         <v>29</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AE7" s="25" t="s">
         <v>11</v>
       </c>
       <c r="AF7" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG7" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AH7" s="5" t="s">
         <v>32</v>
@@ -18266,7 +18263,7 @@
     </row>
     <row r="16" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
       <c r="AC16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -18321,7 +18318,7 @@
         <v>51</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>53</v>
@@ -18338,16 +18335,16 @@
     </row>
     <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>52</v>
@@ -18356,7 +18353,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -18366,23 +18363,23 @@
     </row>
     <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>57</v>
@@ -18394,7 +18391,7 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -18402,7 +18399,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>57</v>
@@ -18414,7 +18411,7 @@
     </row>
     <row r="5" spans="1:10" customFormat="1" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -18422,7 +18419,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>57</v>
@@ -18434,21 +18431,21 @@
     </row>
     <row r="6" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>57</v>
@@ -18580,23 +18577,23 @@
     </row>
     <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -18606,7 +18603,7 @@
     </row>
     <row r="14" spans="1:10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -18614,7 +18611,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>57</v>
@@ -18626,7 +18623,7 @@
     </row>
     <row r="15" spans="1:10" customFormat="1" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -18634,7 +18631,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>57</v>
@@ -18646,21 +18643,21 @@
     </row>
     <row r="16" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>57</v>
@@ -18674,16 +18671,16 @@
     </row>
     <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>230</v>
-      </c>
       <c r="D17" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>52</v>
@@ -18692,7 +18689,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>57</v>
@@ -18729,28 +18726,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>148</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -18811,159 +18808,159 @@
         <v>6</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="M1" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O1" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="X1" s="15" t="s">
-        <v>185</v>
-      </c>
       <c r="Y1" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="Y2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -18976,8 +18973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7161A4-3871-41B8-AFD3-D2E01A42417C}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19001,10 +18998,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -19031,19 +19028,19 @@
         <v>74</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>31</v>
@@ -19059,10 +19056,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>65</v>
@@ -19071,37 +19068,37 @@
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -19109,10 +19106,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>65</v>
@@ -19121,13 +19118,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>72</v>
@@ -19135,20 +19132,20 @@
       <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>75</v>
+      <c r="K3" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P3" s="8"/>
     </row>
@@ -19157,25 +19154,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>72</v>
@@ -19183,20 +19180,20 @@
       <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>75</v>
+      <c r="K4" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P4" s="8"/>
     </row>
@@ -19223,7 +19220,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -19235,7 +19232,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>69</v>
@@ -19249,23 +19246,23 @@
       <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>75</v>
+      <c r="K6" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
@@ -19273,7 +19270,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
@@ -19285,7 +19282,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>69</v>
@@ -19299,23 +19296,23 @@
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>75</v>
+      <c r="K7" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P7" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
@@ -19323,7 +19320,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -19332,10 +19329,10 @@
         <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>69</v>
@@ -19349,23 +19346,23 @@
       <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>75</v>
+      <c r="K8" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -19373,10 +19370,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>65</v>
@@ -19385,13 +19382,13 @@
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>72</v>
@@ -19399,23 +19396,23 @@
       <c r="J9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>75</v>
+      <c r="K9" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -19423,10 +19420,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>65</v>
@@ -19435,37 +19432,37 @@
         <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="O10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
@@ -19473,10 +19470,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>65</v>
@@ -19485,37 +19482,37 @@
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="J11" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="J11" s="28" t="s">
+      <c r="K11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N11" s="28" t="s">
-        <v>220</v>
-      </c>
       <c r="O11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -19523,10 +19520,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>65</v>
@@ -19535,37 +19532,37 @@
         <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="J12" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="28" t="s">
-        <v>220</v>
-      </c>
       <c r="O12" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.3">
@@ -19573,10 +19570,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>65</v>
@@ -19585,37 +19582,37 @@
         <v>10</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I13" s="24" t="s">
         <v>72</v>
       </c>
       <c r="J13" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="K13" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="N13" s="28" t="s">
-        <v>220</v>
-      </c>
       <c r="O13" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.3">
@@ -19623,10 +19620,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>65</v>
@@ -19635,13 +19632,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>72</v>
@@ -19650,19 +19647,19 @@
         <v>11</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L14" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M14" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N14" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P14" s="8"/>
     </row>
@@ -19671,25 +19668,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>72</v>
@@ -19698,19 +19695,19 @@
         <v>11</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M15" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P15" s="8"/>
     </row>
@@ -19719,10 +19716,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>65</v>
@@ -19731,34 +19728,34 @@
         <v>9</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>72</v>
       </c>
       <c r="J16" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="K16" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="M16" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>226</v>
-      </c>
       <c r="O16" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
@@ -19772,10 +19769,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>65</v>
@@ -19784,37 +19781,37 @@
         <v>10</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>72</v>
       </c>
       <c r="J17" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="K17" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="M17" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="N17" s="28" t="s">
-        <v>220</v>
-      </c>
       <c r="O17" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -19860,58 +19857,58 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="O1" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>205</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -19925,40 +19922,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -19966,22 +19963,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -19989,22 +19986,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
@@ -20012,22 +20009,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -20035,27 +20032,27 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="G9" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
28 Dec Changes done
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BuildPiperTestData.xlsx
+++ b/src/test/resources/testdata/BuildPiperTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4933ECED-9F07-4313-8A4F-A2DF61228C04}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{380C24BE-CC61-4AF2-B729-2343E611FF30}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15564" windowHeight="3360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12912" windowHeight="3528" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="RepoIntegrationData" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="AA1:AE5"/>
+  <oleSize ref="K12:P21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="246">
   <si>
     <t>username</t>
   </si>
@@ -762,6 +762,9 @@
   </si>
   <si>
     <t>HPAOtherDeploymentInfo</t>
+  </si>
+  <si>
+    <t>EditPipeline</t>
   </si>
 </sst>
 </file>
@@ -1384,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33546052-E966-4F68-882D-901C990EE3E6}">
   <dimension ref="A1:XFD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19036,10 +19039,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7161A4-3871-41B8-AFD3-D2E01A42417C}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="K12" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19903,6 +19906,56 @@
         <v>242</v>
       </c>
       <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>1</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="28">
+        <v>10</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N19" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="O19" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>